<commit_message>
Completed analysis of matching between waswordt and definitietabel with waswordt versionJakko
</commit_message>
<xml_diff>
--- a/data/dt_cleaned.xlsx
+++ b/data/dt_cleaned.xlsx
@@ -11125,7 +11125,7 @@
       <c r="H238" t="inlineStr"/>
       <c r="I238" t="inlineStr"/>
       <c r="J238" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K238" t="b">
         <v>0</v>
@@ -13461,7 +13461,7 @@
       <c r="H290" t="inlineStr"/>
       <c r="I290" t="inlineStr"/>
       <c r="J290" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K290" t="b">
         <v>0</v>
@@ -13506,7 +13506,7 @@
       </c>
       <c r="I291" t="inlineStr"/>
       <c r="J291" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K291" t="b">
         <v>0</v>
@@ -18955,7 +18955,7 @@
       </c>
       <c r="I412" t="inlineStr"/>
       <c r="J412" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K412" t="b">
         <v>0</v>
@@ -19000,7 +19000,7 @@
       </c>
       <c r="I413" t="inlineStr"/>
       <c r="J413" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K413" t="b">
         <v>0</v>
@@ -19045,7 +19045,7 @@
       </c>
       <c r="I414" t="inlineStr"/>
       <c r="J414" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K414" t="b">
         <v>0</v>
@@ -19090,7 +19090,7 @@
       </c>
       <c r="I415" t="inlineStr"/>
       <c r="J415" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K415" t="b">
         <v>0</v>
@@ -22968,7 +22968,7 @@
       <c r="H501" t="inlineStr"/>
       <c r="I501" t="inlineStr"/>
       <c r="J501" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K501" t="b">
         <v>0</v>
@@ -23058,7 +23058,7 @@
       <c r="H503" t="inlineStr"/>
       <c r="I503" t="inlineStr"/>
       <c r="J503" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K503" t="b">
         <v>0</v>
@@ -23103,7 +23103,7 @@
       <c r="H504" t="inlineStr"/>
       <c r="I504" t="inlineStr"/>
       <c r="J504" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K504" t="b">
         <v>0</v>
@@ -25082,7 +25082,7 @@
         <v>0</v>
       </c>
       <c r="K548" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="549">
@@ -25217,7 +25217,7 @@
         <v>0</v>
       </c>
       <c r="K551" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="552">
@@ -28363,7 +28363,7 @@
         <v>0</v>
       </c>
       <c r="K621" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="622">
@@ -28723,7 +28723,7 @@
         <v>0</v>
       </c>
       <c r="K629" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="630">
@@ -28768,7 +28768,7 @@
         <v>0</v>
       </c>
       <c r="K630" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="631">
@@ -28813,7 +28813,7 @@
         <v>0</v>
       </c>
       <c r="K631" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="632">
@@ -28858,7 +28858,7 @@
         <v>0</v>
       </c>
       <c r="K632" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="633">
@@ -28903,7 +28903,7 @@
         <v>0</v>
       </c>
       <c r="K633" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="634">
@@ -28948,7 +28948,7 @@
         <v>0</v>
       </c>
       <c r="K634" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>